<commit_message>
update part and get_pond statements
</commit_message>
<xml_diff>
--- a/pond2/generator/gene_data.xlsx
+++ b/pond2/generator/gene_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\pond2\pond2\generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\pond2\pond2\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17194" windowHeight="6190"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="17190" windowHeight="6195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,73 +24,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
   <si>
     <t>total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>LINE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PART_OS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PART_DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thick_clg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sym_flt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asym_flt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flt_ro1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flt_ro5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flt_ro3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_COUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PART_CL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>SEGMENT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LINE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>thick_ct</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CALC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>all</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ITEM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PART_CL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>thick_ct</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>thick</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PART_OS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PART_DS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P_COUNT</t>
+    <t>HD_LEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TL_LEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UPPER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HD_LEN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TL_LEN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -124,12 +160,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,11 +200,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,107 +496,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D2" sqref="D2:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="5" width="11" customWidth="1"/>
-    <col min="7" max="7" width="9.69921875" customWidth="1"/>
-    <col min="9" max="9" width="8.296875" customWidth="1"/>
-    <col min="10" max="10" width="9.8984375" customWidth="1"/>
+    <col min="4" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="9.75" customWidth="1"/>
+    <col min="9" max="9" width="8.25" customWidth="1"/>
+    <col min="10" max="10" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
+        <v>1580</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="4">
+        <v>2250</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>1580</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6</v>
+      </c>
+      <c r="J4" s="2">
+        <v>6</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>1580</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>1580</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2">
+        <v>6</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>1580</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="I7" s="2">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>2250</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="3">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>2250</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="3">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3">
+        <v>6</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>2250</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>1580</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3">
+        <v>6</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>2250</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
-        <v>2250</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="3">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3">
+        <v>6</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start to do sth with flatness
</commit_message>
<xml_diff>
--- a/pond2/generator/gene_data.xlsx
+++ b/pond2/generator/gene_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="0" windowWidth="17190" windowHeight="6195"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="17190" windowHeight="6195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="85">
   <si>
     <t>total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -282,6 +282,71 @@
   </si>
   <si>
     <t>thick_0.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shift_f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shift_f2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shift_f3</t>
+  </si>
+  <si>
+    <t>shift_f4</t>
+  </si>
+  <si>
+    <t>shift_f5</t>
+  </si>
+  <si>
+    <t>shift_f6</t>
+  </si>
+  <si>
+    <t>shift_f7</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos_shft_f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos_shft_f2</t>
+  </si>
+  <si>
+    <t>pos_shft_f3</t>
+  </si>
+  <si>
+    <t>pos_shft_f4</t>
+  </si>
+  <si>
+    <t>pos_shft_f5</t>
+  </si>
+  <si>
+    <t>pos_shft_f6</t>
+  </si>
+  <si>
+    <t>pos_shft_f7</t>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -315,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +429,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -379,7 +450,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -405,6 +476,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -687,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1218,7 +1295,7 @@
         <v>47</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>29</v>
@@ -2323,7 +2400,7 @@
         <v>56</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="I43" s="4">
         <v>2</v>
@@ -2565,6 +2642,541 @@
       <c r="L49" s="8">
         <v>16</v>
       </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A50" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="10">
+        <v>1</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I50" s="10">
+        <v>2</v>
+      </c>
+      <c r="J50" s="10">
+        <v>2</v>
+      </c>
+      <c r="K50" s="10">
+        <v>0</v>
+      </c>
+      <c r="L50" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A51" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="10">
+        <v>1</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I51" s="10">
+        <v>2</v>
+      </c>
+      <c r="J51" s="10">
+        <v>2</v>
+      </c>
+      <c r="K51" s="10">
+        <v>0</v>
+      </c>
+      <c r="L51" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A52" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="10">
+        <v>1</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I52" s="10">
+        <v>2</v>
+      </c>
+      <c r="J52" s="10">
+        <v>2</v>
+      </c>
+      <c r="K52" s="10">
+        <v>0</v>
+      </c>
+      <c r="L52" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A53" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="10">
+        <v>1</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I53" s="10">
+        <v>2</v>
+      </c>
+      <c r="J53" s="10">
+        <v>2</v>
+      </c>
+      <c r="K53" s="10">
+        <v>0</v>
+      </c>
+      <c r="L53" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A54" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="10">
+        <v>1</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I54" s="10">
+        <v>2</v>
+      </c>
+      <c r="J54" s="10">
+        <v>2</v>
+      </c>
+      <c r="K54" s="10">
+        <v>0</v>
+      </c>
+      <c r="L54" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A55" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="10">
+        <v>1</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I55" s="10">
+        <v>2</v>
+      </c>
+      <c r="J55" s="10">
+        <v>2</v>
+      </c>
+      <c r="K55" s="10">
+        <v>0</v>
+      </c>
+      <c r="L55" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A56" s="10">
+        <v>1580</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="10">
+        <v>1</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I56" s="10">
+        <v>2</v>
+      </c>
+      <c r="J56" s="10">
+        <v>2</v>
+      </c>
+      <c r="K56" s="10">
+        <v>0</v>
+      </c>
+      <c r="L56" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A57" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="10">
+        <v>1</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I57" s="10">
+        <v>2</v>
+      </c>
+      <c r="J57" s="10">
+        <v>2</v>
+      </c>
+      <c r="K57" s="10">
+        <v>0</v>
+      </c>
+      <c r="L57" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A58" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="10">
+        <v>1</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I58" s="10">
+        <v>2</v>
+      </c>
+      <c r="J58" s="10">
+        <v>2</v>
+      </c>
+      <c r="K58" s="10">
+        <v>0</v>
+      </c>
+      <c r="L58" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A59" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="10">
+        <v>1</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I59" s="10">
+        <v>2</v>
+      </c>
+      <c r="J59" s="10">
+        <v>2</v>
+      </c>
+      <c r="K59" s="10">
+        <v>0</v>
+      </c>
+      <c r="L59" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A60" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="10">
+        <v>1</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I60" s="10">
+        <v>2</v>
+      </c>
+      <c r="J60" s="10">
+        <v>2</v>
+      </c>
+      <c r="K60" s="10">
+        <v>0</v>
+      </c>
+      <c r="L60" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A61" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="10">
+        <v>1</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I61" s="10">
+        <v>2</v>
+      </c>
+      <c r="J61" s="10">
+        <v>2</v>
+      </c>
+      <c r="K61" s="10">
+        <v>0</v>
+      </c>
+      <c r="L61" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A62" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="10">
+        <v>1</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I62" s="10">
+        <v>2</v>
+      </c>
+      <c r="J62" s="10">
+        <v>2</v>
+      </c>
+      <c r="K62" s="10">
+        <v>0</v>
+      </c>
+      <c r="L62" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A63" s="10">
+        <v>2250</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="10">
+        <v>1</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I63" s="10">
+        <v>2</v>
+      </c>
+      <c r="J63" s="10">
+        <v>2</v>
+      </c>
+      <c r="K63" s="10">
+        <v>0</v>
+      </c>
+      <c r="L63" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A64" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>